<commit_message>
remove - innecesary stuff
</commit_message>
<xml_diff>
--- a/Projects/UNA/Asesoría Jmeter/PlanificaciónDeSesiones.xlsx
+++ b/Projects/UNA/Asesoría Jmeter/PlanificaciónDeSesiones.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Avantica\Projects\UNA\Asesoría Jmeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Avantica\Projects\UNA\Asesoría Jmeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="8655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="8655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Sesion 1</t>
   </si>
@@ -198,12 +199,54 @@
   </si>
   <si>
     <t>Nota: En esta sesion se pretende que el personal de la UNA sea capaz de desarrollar scripts dinamicos y corregir los scripts que han desarrollado hasta el momento.</t>
+  </si>
+  <si>
+    <t>Temas</t>
+  </si>
+  <si>
+    <t>Sesion</t>
+  </si>
+  <si>
+    <t>Estimado</t>
+  </si>
+  <si>
+    <t>Conceptos Basicos</t>
+  </si>
+  <si>
+    <t>Introduccion a Jmeter</t>
+  </si>
+  <si>
+    <t>Instalacion de Jmeter</t>
+  </si>
+  <si>
+    <t>Plugins Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recording </t>
+  </si>
+  <si>
+    <t>Configuración de CSV Data set</t>
+  </si>
+  <si>
+    <t>Expresiones regulares</t>
+  </si>
+  <si>
+    <t>Jmeter funciones</t>
+  </si>
+  <si>
+    <t>Ejecucion de pruebas</t>
+  </si>
+  <si>
+    <t>Analisis de resultados</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -272,6 +315,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,4 +1226,107 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>